<commit_message>
added mobile changes refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FL\test-crew-automation\testcrew-parent-framework-light\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FL\test-crew-automation\WebAPIFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41774FEF-98D9-4141-8C90-D27DB5E94F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E68F62-F25C-4C1F-82E9-94F6D37C2A1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,11 @@
     <sheet name="Flipkart" sheetId="3" r:id="rId3"/>
     <sheet name="Typicode" sheetId="4" r:id="rId4"/>
     <sheet name="DemoSite" sheetId="6" r:id="rId5"/>
+    <sheet name="Mobile" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>P_Key</t>
   </si>
@@ -167,12 +168,49 @@
   </si>
   <si>
     <t>typiCodeApiGetTestRawUse</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>swagLoginTest</t>
+  </si>
+  <si>
+    <t>Swag Mobile app test</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>testFirstName</t>
+  </si>
+  <si>
+    <t>testLastName</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +330,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -573,20 +614,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -649,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -674,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -710,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -746,7 +787,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -782,7 +823,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -798,7 +839,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>17</v>
@@ -807,7 +848,7 @@
         <v>44</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -823,16 +864,55 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E11" xr:uid="{6941C086-FDEB-4E3E-9B5A-A6454B855CFD}">
-      <formula1>"Web,Api,Mix"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:H13 G3:H11" xr:uid="{C0793967-8806-4E94-BDD5-948D00322585}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H11" xr:uid="{C0793967-8806-4E94-BDD5-948D00322585}">
-      <formula1>"Yes,No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{319365FA-5F26-42A7-9A4E-5B32396C3CA9}">
+      <formula1>"Web,Api,Web-Api,Mobile"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -844,10 +924,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -935,6 +1015,7 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{59395D6D-FB57-43DD-BCC4-DFC92ED7351B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -946,10 +1027,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,6 +1086,7 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{9242CDDA-A551-41BC-9FD8-99A8EF6882B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1016,10 +1098,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,6 +1148,7 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{3F8E1370-6F75-4575-8805-12D5037E1C61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1077,12 +1160,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,5 +1211,75 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{112122F0-E10A-4360-A3E4-03663921DB29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1504A0-8417-4DF0-B4F2-1E007ED88E7B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="2">
+        <v>94025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting appium from framework
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
   <si>
     <t>P_Key</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>

</xml_diff>